<commit_message>
some updates for WS23 modules
</commit_message>
<xml_diff>
--- a/KurseMscECMX_WiSe23.xlsx
+++ b/KurseMscECMX_WiSe23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/git_projects/CourseOverview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F6B183-3636-E84E-8CF8-E16A5FE53724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82B472E-F8BF-7542-93D3-3F60CE5FE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10280" yWindow="5480" windowWidth="30240" windowHeight="19000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3308,10 +3308,10 @@
   <dimension ref="A1:AMD125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A117" sqref="A117"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -4054,7 +4054,7 @@
         <v>409</v>
       </c>
       <c r="I20" s="25">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>11</v>

</xml_diff>